<commit_message>
28/09/17 - Comienza seccion acceso cliente, para ver estado de la tramitacion
</commit_message>
<xml_diff>
--- a/htdocs/App/Controllers/Traspasos/5080CNW.xlsx
+++ b/htdocs/App/Controllers/Traspasos/5080CNW.xlsx
@@ -31,25 +31,25 @@
     <t>Fecha Entrada</t>
   </si>
   <si>
-    <t>2017-08-31 14:04:37</t>
+    <t>14-09-2017</t>
   </si>
   <si>
     <t>Atendido por:</t>
   </si>
   <si>
-    <t>Admin</t>
+    <t>Jaume</t>
   </si>
   <si>
     <t>Provisión</t>
   </si>
   <si>
-    <t>efectivo</t>
+    <t>visa</t>
   </si>
   <si>
     <t>Cobrado el</t>
   </si>
   <si>
-    <t>2017-08-31</t>
+    <t>2017-09-14</t>
   </si>
   <si>
     <t>x</t>
@@ -64,7 +64,7 @@
     <t>Vendedor:</t>
   </si>
   <si>
-    <t>STEFAN CONSTANTIN SOTIR</t>
+    <t>ANAMARIA MARIN</t>
   </si>
   <si>
     <t>Impresos/Fotocopias…………………….</t>
@@ -97,7 +97,7 @@
     <t>Comprador:</t>
   </si>
   <si>
-    <t>ANAMARIA MARIN</t>
+    <t>RAFAEL BAZAN</t>
   </si>
   <si>
     <t>Pago y Gest. IVTM………………</t>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C16" s="44"/>
       <c r="D16" s="73">
-        <v>603178416</v>
+        <v>672576947</v>
       </c>
       <c r="E16" s="73"/>
       <c r="F16" s="73"/>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="73">
-        <v>672576947</v>
+        <v>604108239</v>
       </c>
       <c r="E23" s="73"/>
       <c r="F23" s="73"/>

</xml_diff>